<commit_message>
New Diagram and Tables
</commit_message>
<xml_diff>
--- a/RegistroTareas.xlsx
+++ b/RegistroTareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aef0bc37a74e6c06/Escritorio/Ingenieria Curso 4/ISO/appTurismo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedrobereilh/Desktop/appTurismo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="11_FC1EA42D3D9A42F180441987ADCACBFB7E6597A9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48176741-27A3-4D9C-AC25-8C0CC132E427}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4894CBCB-7211-CA44-92A6-F64062C4977F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="43">
   <si>
     <t>ID Requisito</t>
   </si>
@@ -150,6 +150,18 @@
   </si>
   <si>
     <t>Asignación de etiquetas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear Diagrama </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear Tablas Base de Datos </t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>EN PROCESO</t>
   </si>
 </sst>
 </file>
@@ -205,12 +217,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -478,23 +493,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="38.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +535,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>21</v>
       </c>
@@ -545,7 +560,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>21</v>
       </c>
@@ -570,7 +585,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>21</v>
       </c>
@@ -595,7 +610,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>21</v>
       </c>
@@ -620,7 +635,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>21</v>
       </c>
@@ -643,7 +658,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>21</v>
       </c>
@@ -668,7 +683,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>21</v>
       </c>
@@ -693,7 +708,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>21</v>
       </c>
@@ -718,7 +733,7 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -745,7 +760,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>22</v>
       </c>
@@ -768,7 +783,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>22</v>
       </c>
@@ -791,7 +806,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -818,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>25</v>
       </c>
@@ -843,7 +858,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>25</v>
       </c>
@@ -866,7 +881,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>25</v>
       </c>
@@ -889,7 +904,7 @@
       </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>25</v>
       </c>
@@ -912,7 +927,7 @@
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
         <v>25</v>
       </c>
@@ -935,7 +950,7 @@
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -962,7 +977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
         <v>10</v>
       </c>
@@ -987,7 +1002,7 @@
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
         <v>10</v>
       </c>
@@ -1012,7 +1027,7 @@
       </c>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
         <v>10</v>
       </c>
@@ -1035,7 +1050,7 @@
       </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
         <v>10</v>
       </c>
@@ -1058,7 +1073,7 @@
       </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
         <v>10</v>
       </c>
@@ -1081,7 +1096,7 @@
       </c>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -1108,7 +1123,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
         <v>45</v>
       </c>
@@ -1133,7 +1148,7 @@
       </c>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
         <v>45</v>
       </c>
@@ -1158,7 +1173,7 @@
       </c>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1">
         <v>45</v>
       </c>
@@ -1183,7 +1198,7 @@
       </c>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1">
         <v>45</v>
       </c>
@@ -1208,7 +1223,7 @@
       </c>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>18</v>
       </c>
@@ -1235,7 +1250,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -1258,7 +1273,7 @@
       </c>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -1281,7 +1296,7 @@
       </c>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1">
         <v>1</v>
       </c>
@@ -1304,7 +1319,7 @@
       </c>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1">
         <v>1</v>
       </c>
@@ -1327,7 +1342,7 @@
       </c>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>18</v>
       </c>
@@ -1352,6 +1367,42 @@
       <c r="H35" s="2">
         <f>SUM(D31:D34)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B42" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="3">
+        <v>2</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B43" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="3">
+        <v>2</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>